<commit_message>
Add note about output oddity
</commit_message>
<xml_diff>
--- a/materials/rwe-eeg_s1_r1_e1/resources/passageList.xlsx
+++ b/materials/rwe-eeg_s1_r1_e1/resources/passageList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jalexand/github/rwe-eeg-dataset/materials/rwe-eeg_s1_r1_e1/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCE8C40-2E0A-1643-AE7F-6CDBA014DBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F94218-FED0-2945-8B2D-10C4E2A6D41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="29160" windowHeight="15020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1077,7 +1077,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>